<commit_message>
Added match education feature
</commit_message>
<xml_diff>
--- a/DocumentProcessing/Output_Folder/matchingResults 28May2021.xlsx
+++ b/DocumentProcessing/Output_Folder/matchingResults 28May2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\Personal\UiPath\RPA-J-01 Job matching for Placements\DocumentProcessing\Output_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1273E02-C411-44DD-BEA7-F40EE715156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DE7A59-E315-4ACD-8A90-9034030F59A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="3375" windowWidth="23070" windowHeight="15345" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="0" yWindow="3375" windowWidth="32280" windowHeight="15345" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="CandidateMatching" sheetId="2" r:id="rId1"/>
@@ -57,25 +57,30 @@
     <x:t>abiral.pandey88@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">bachelor </x:t>
+    <x:t>bachelor</x:t>
   </x:si>
   <x:si>
     <x:t>design,technical,reporting,documentation,content,database,testing,writing,programming,agile,architecture,troubleshooting,computer science,automation,sql,installation,windows,frameworks,bi,html,software development,oracle,java,business process,pr,javascript,linux,life cycle,cad,css,e-commerce,cloud,technical skills,operating systems,sas,ux,end user,analysis,sdlc,aws,jira,test plans,ui,front-end,api,ibm,scripting,mis,os,etl,test cases,lan,sci,unix,web services,software development life cycle,sql server,html5</x:t>
   </x:si>
   <x:si>
-    <x:t>51.72%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>37.29%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>46.67%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>41.38%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36.73%</x:t>
+    <x:t>51.72% matched
+Education :Met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>37.29% matched
+Education :Met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46.67% matched
+Education :Met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41.38% matched
+Education :Met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36.73% matched
+Education :Met</x:t>
   </x:si>
   <x:si>
     <x:t>Achyuth Resume_8</x:t>
@@ -87,16 +92,20 @@
     <x:t>design,operations,technical,reporting,engineering,policies,health,customer service,content,presentation,database,testing,writing,healthcare,programming,agile,architecture,automation,modeling,sql,payments,lean,transactions,windows,banking,business requirements,technical support,frameworks,bi,html,software development,oracle,java,erp,pr,javascript,linux,life cycle,cad,css,ecommerce,c++,cloud,python,technical skills,workflows,intranet,ux,mortgage,analysis,sdlc,aws,jira,usability,ui,api,ibm,scripting,os,apis,test cases,prototype,lan,unix,web services,software development life cycle,sql server,small business,html5</x:t>
   </x:si>
   <x:si>
-    <x:t>55.17%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40.68%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36.67%</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40.82%</x:t>
+    <x:t>55.17% matched
+Education :Not met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40.68% matched
+Education :Not met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36.67% matched
+Education :Not met</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40.82% matched
+Education :Not met</x:t>
   </x:si>
   <x:si>
     <x:t>JD Title</x:t>
@@ -185,8 +194,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment wrapText="1"/>
@@ -522,104 +530,170 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I3"/>
+  <x:dimension ref="A1:D14"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <x:selection activeCell="E1" sqref="E1 E1:J1048576"/>
+      <x:selection activeCell="E1" sqref="E1 E1:I1048576"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="20.285156" style="8" customWidth="1"/>
-    <x:col min="2" max="2" width="29.855469" style="8" customWidth="1"/>
-    <x:col min="3" max="3" width="20.570312" style="8" customWidth="1"/>
-    <x:col min="4" max="4" width="109.140625" style="8" customWidth="1"/>
+    <x:col min="1" max="1" width="20.285156" style="7" customWidth="1"/>
+    <x:col min="2" max="2" width="29.855469" style="7" customWidth="1"/>
+    <x:col min="3" max="3" width="20.570312" style="7" customWidth="1"/>
+    <x:col min="4" max="4" width="109.140625" style="7" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="7" t="s">
+      <x:c r="A1" s="6" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="7" t="s">
+      <x:c r="B1" s="6" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="7" t="s">
+      <x:c r="C1" s="6" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="7" t="s">
+      <x:c r="D1" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="6" t="s">
+      <x:c r="E1" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="6" t="s">
+      <x:c r="F1" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="6" t="s">
+      <x:c r="G1" s="5" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="6" t="s">
+      <x:c r="H1" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="6" t="s">
+      <x:c r="I1" s="5" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:9" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="7" t="s">
+    <x:row r="2" spans="1:9" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="6" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B2" s="7" t="s">
+      <x:c r="B2" s="6" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C2" s="7" t="s">
+      <x:c r="C2" s="6" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D2" s="7" t="s">
+      <x:c r="D2" s="6" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E2" s="6" t="s">
+      <x:c r="E2" s="7" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="F2" s="6" t="s">
+      <x:c r="F2" s="7" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="G2" s="6" t="s">
+      <x:c r="G2" s="7" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="H2" s="6" t="s">
+      <x:c r="H2" s="7" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I2" s="6" t="s">
+      <x:c r="I2" s="7" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:9" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="7" t="s">
+      <x:c r="A3" s="6" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="B3" s="7" t="s">
+      <x:c r="B3" s="6" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C3" s="7" t="s"/>
-      <x:c r="D3" s="7" t="s">
+      <x:c r="C3" s="6" t="s"/>
+      <x:c r="D3" s="6" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="E3" s="6" t="s">
+      <x:c r="E3" s="7" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="F3" s="6" t="s">
+      <x:c r="F3" s="7" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="G3" s="6" t="s">
+      <x:c r="G3" s="7" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="H3" s="6" t="s">
+      <x:c r="H3" s="7" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="I3" s="6" t="s">
+      <x:c r="I3" s="7" t="s">
         <x:v>24</x:v>
       </x:c>
+    </x:row>
+    <x:row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="6" t="s"/>
+      <x:c r="B4" s="6" t="s"/>
+      <x:c r="C4" s="6" t="s"/>
+      <x:c r="D4" s="6" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="6" t="s"/>
+      <x:c r="B5" s="6" t="s"/>
+      <x:c r="C5" s="6" t="s"/>
+      <x:c r="D5" s="6" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="6" t="s"/>
+      <x:c r="B6" s="6" t="s"/>
+      <x:c r="C6" s="6" t="s"/>
+      <x:c r="D6" s="6" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="6" t="s"/>
+      <x:c r="B7" s="6" t="s"/>
+      <x:c r="C7" s="6" t="s"/>
+      <x:c r="D7" s="6" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="6" t="s"/>
+      <x:c r="B8" s="6" t="s"/>
+      <x:c r="C8" s="6" t="s"/>
+      <x:c r="D8" s="6" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="6" t="s"/>
+      <x:c r="B9" s="6" t="s"/>
+      <x:c r="C9" s="6" t="s"/>
+      <x:c r="D9" s="6" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="6" t="s"/>
+      <x:c r="B10" s="6" t="s"/>
+      <x:c r="C10" s="6" t="s"/>
+      <x:c r="D10" s="6" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="6" t="s"/>
+      <x:c r="B11" s="6" t="s"/>
+      <x:c r="C11" s="6" t="s"/>
+      <x:c r="D11" s="6" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="6" t="s"/>
+      <x:c r="B12" s="6" t="s"/>
+      <x:c r="C12" s="6" t="s"/>
+      <x:c r="D12" s="6" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A13" s="6" t="s"/>
+      <x:c r="B13" s="6" t="s"/>
+      <x:c r="C13" s="6" t="s"/>
+      <x:c r="D13" s="6" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <x:c r="A14" s="6" t="s"/>
+      <x:c r="B14" s="6" t="s"/>
+      <x:c r="C14" s="6" t="s"/>
+      <x:c r="D14" s="6" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -638,82 +712,85 @@
   <x:dimension ref="A1:E6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="H5" sqref="H5 H5:H5"/>
+      <x:selection activeCell="B16" sqref="B16 B16:B16"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="19" style="7" customWidth="1"/>
-    <x:col min="2" max="2" width="33.710938" style="7" customWidth="1"/>
-    <x:col min="3" max="3" width="110" style="7" customWidth="1"/>
-    <x:col min="4" max="5" width="9.140625" style="10" customWidth="1"/>
+    <x:col min="1" max="1" width="19" style="6" customWidth="1"/>
+    <x:col min="2" max="2" width="33.710938" style="6" customWidth="1"/>
+    <x:col min="3" max="3" width="110" style="6" customWidth="1"/>
+    <x:col min="4" max="5" width="9.140625" style="9" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="9" t="s">
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="8" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B1" s="9" t="s">
+      <x:c r="B1" s="8" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C1" s="9" t="s">
+      <x:c r="C1" s="8" t="s">
         <x:v>27</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:8" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+    <x:row r="2" spans="1:5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="8" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="8" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C2" s="9" t="s">
+      <x:c r="C2" s="8" t="s">
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:8" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="s">
+    <x:row r="3" spans="1:5" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="8" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="8" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C3" s="9" t="s">
+      <x:c r="C3" s="8" t="s">
         <x:v>30</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:8" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="9" t="s">
+    <x:row r="4" spans="1:5" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="8" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B4" s="9" t="s">
+      <x:c r="B4" s="8" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="C4" s="9" t="s">
+      <x:c r="C4" s="8" t="s">
         <x:v>32</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:8" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="9" t="s">
+    <x:row r="5" spans="1:5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="8" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B5" s="9" t="s">
+      <x:c r="B5" s="8" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C5" s="9" t="s">
+      <x:c r="C5" s="8" t="s">
         <x:v>33</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:8" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="9" t="s">
+    <x:row r="6" spans="1:5" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="8" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B6" s="9" t="s">
+      <x:c r="B6" s="8" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="C6" s="9" t="s">
+      <x:c r="C6" s="8" t="s">
         <x:v>35</x:v>
       </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="B16" s="6" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>